<commit_message>
Sigi-12: Update coordinates for the test seals in Excel
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/test.xlsx
+++ b/ExcelToXMLConverter/resources/test.xlsx
@@ -376,10 +376,10 @@
     <t xml:space="preserve">COORDINATES</t>
   </si>
   <si>
-    <t xml:space="preserve">42.136897, 24.742168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.697334, 23.325941</t>
+    <t xml:space="preserve">42.186897, 24.742168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42.707334, 23.325941</t>
   </si>
   <si>
     <t xml:space="preserve">FIND DATE</t>
@@ -905,11 +905,11 @@
   </sheetPr>
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="60.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.85"/>
@@ -1487,7 +1487,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>

</xml_diff>